<commit_message>
login, show file list for download complete
</commit_message>
<xml_diff>
--- a/backend/exports/202407.xlsx
+++ b/backend/exports/202407.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="テスト111111" sheetId="1" r:id="rId1"/>
+    <sheet name="テスト123456" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -415,29 +415,18 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>202473</v>
+        <v>20240708</v>
       </c>
       <c r="B2" t="str">
         <v>0/100</v>
       </c>
       <c r="C2" t="str">
-        <v>00:02</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>202473</v>
-      </c>
-      <c r="B3" t="str">
-        <v>0/100</v>
-      </c>
-      <c r="C3" t="str">
         <v>00:02</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>